<commit_message>
Add vectorized 2015 and 2020 dataset + some cleaning
</commit_message>
<xml_diff>
--- a/data/BDD.xlsx
+++ b/data/BDD.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\charl\solar-data-china\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F17C1937-168A-4A71-9432-0C3ECBB414D5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5E5FDB03-8EE5-43C7-8BA7-D587E84CD757}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Dataset" sheetId="1" r:id="rId1"/>
@@ -1040,7 +1040,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="62">
+  <cellXfs count="54">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -1186,29 +1186,7 @@
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="1"/>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1217,6 +1195,37 @@
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="38">
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="8"/>
+      </font>
+      <fill>
+        <patternFill>
+          <fgColor theme="6"/>
+          <bgColor theme="6" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <strike val="0"/>
@@ -1435,37 +1444,6 @@
         <patternFill patternType="none">
           <fgColor indexed="64"/>
           <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="8"/>
-      </font>
-      <fill>
-        <patternFill>
-          <fgColor theme="6"/>
-          <bgColor theme="6" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
         </patternFill>
       </fill>
     </dxf>
@@ -1706,18 +1684,18 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{00000000-000C-0000-FFFF-FFFF01000000}" name="Articles" displayName="Articles" ref="A1:J30" headerRowDxfId="12" dataDxfId="11" totalsRowDxfId="10">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{00000000-000C-0000-FFFF-FFFF01000000}" name="Articles" displayName="Articles" ref="A1:J30" headerRowDxfId="15" dataDxfId="14" totalsRowDxfId="13">
   <tableColumns count="10">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0100-000001000000}" name="Title " dataDxfId="9"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0100-000002000000}" name="Author " dataDxfId="8"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0100-000003000000}" name="Date " dataDxfId="7"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0100-000004000000}" name="Journal /preprint" dataDxfId="6"/>
-    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0100-000005000000}" name="Link" dataDxfId="5"/>
-    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0100-000006000000}" name="Summary " dataDxfId="4"/>
-    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0100-000007000000}" name="Methodology" dataDxfId="3"/>
-    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0100-000008000000}" name="Dataset" dataDxfId="2"/>
-    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0100-000009000000}" name="Coverage" dataDxfId="1"/>
-    <tableColumn id="10" xr3:uid="{00000000-0010-0000-0100-00000A000000}" name="Notes " dataDxfId="0"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0100-000001000000}" name="Title " dataDxfId="12"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0100-000002000000}" name="Author " dataDxfId="11"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0100-000003000000}" name="Date " dataDxfId="10"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0100-000004000000}" name="Journal /preprint" dataDxfId="9"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0100-000005000000}" name="Link" dataDxfId="8"/>
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0100-000006000000}" name="Summary " dataDxfId="7"/>
+    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0100-000007000000}" name="Methodology" dataDxfId="6"/>
+    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0100-000008000000}" name="Dataset" dataDxfId="5"/>
+    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0100-000009000000}" name="Coverage" dataDxfId="4"/>
+    <tableColumn id="10" xr3:uid="{00000000-0010-0000-0100-00000A000000}" name="Notes " dataDxfId="3"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight15" showFirstColumn="1" showLastColumn="1" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1926,7 +1904,7 @@
   </sheetPr>
   <dimension ref="A1:O47"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="66" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScale="66" zoomScaleNormal="100" workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B16" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
@@ -2149,7 +2127,7 @@
       </c>
       <c r="O5" s="18"/>
     </row>
-    <row r="6" spans="1:15" ht="198">
+    <row r="6" spans="1:15" ht="184.8">
       <c r="A6" s="2" t="s">
         <v>35</v>
       </c>
@@ -2781,13 +2759,13 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="L1:L1048576">
-    <cfRule type="cellIs" dxfId="15" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="2" priority="1" operator="equal">
       <formula>"High"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="14" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="1" priority="2" operator="equal">
       <formula>"Medium"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="13" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="0" priority="3" operator="equal">
       <formula>"Low"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -2821,9 +2799,9 @@
   </sheetPr>
   <dimension ref="A1:L1002"/>
   <sheetViews>
-    <sheetView topLeftCell="A23" zoomScale="76" zoomScaleNormal="106" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A3" zoomScale="76" zoomScaleNormal="106" workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="B44" sqref="B44"/>
+      <selection pane="topRight" activeCell="F3" sqref="F3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1"/>
@@ -3021,7 +2999,7 @@
       </c>
       <c r="F7" s="11"/>
       <c r="G7" s="11"/>
-      <c r="H7" s="60" t="s">
+      <c r="H7" s="53" t="s">
         <v>147</v>
       </c>
       <c r="I7" s="42"/>
@@ -3183,7 +3161,7 @@
       <c r="I17" s="42"/>
       <c r="J17" s="11"/>
     </row>
-    <row r="18" spans="1:10" ht="52.8">
+    <row r="18" spans="1:10" ht="39.6">
       <c r="A18" s="50" t="s">
         <v>156</v>
       </c>
@@ -3290,90 +3268,90 @@
       <c r="J24" s="11"/>
     </row>
     <row r="25" spans="1:10" ht="26.4">
-      <c r="A25" s="53" t="s">
+      <c r="A25" s="29" t="s">
         <v>169</v>
       </c>
-      <c r="B25" s="54"/>
-      <c r="C25" s="55"/>
-      <c r="D25" s="56"/>
-      <c r="E25" s="57"/>
-      <c r="F25" s="58"/>
-      <c r="G25" s="58"/>
-      <c r="H25" s="61"/>
-      <c r="I25" s="59"/>
-      <c r="J25" s="58"/>
+      <c r="B25" s="3"/>
+      <c r="C25" s="43"/>
+      <c r="D25" s="1"/>
+      <c r="E25" s="48"/>
+      <c r="F25" s="11"/>
+      <c r="G25" s="11"/>
+      <c r="H25" s="17"/>
+      <c r="I25" s="42"/>
+      <c r="J25" s="11"/>
     </row>
     <row r="26" spans="1:10" ht="39.6">
-      <c r="A26" s="53" t="s">
+      <c r="A26" s="29" t="s">
         <v>170</v>
       </c>
-      <c r="B26" s="54"/>
-      <c r="C26" s="55"/>
-      <c r="D26" s="56"/>
-      <c r="E26" s="57"/>
-      <c r="F26" s="58"/>
-      <c r="G26" s="58"/>
-      <c r="H26" s="61"/>
-      <c r="I26" s="59"/>
-      <c r="J26" s="58"/>
+      <c r="B26" s="3"/>
+      <c r="C26" s="43"/>
+      <c r="D26" s="1"/>
+      <c r="E26" s="48"/>
+      <c r="F26" s="11"/>
+      <c r="G26" s="11"/>
+      <c r="H26" s="17"/>
+      <c r="I26" s="42"/>
+      <c r="J26" s="11"/>
     </row>
     <row r="27" spans="1:10" ht="52.8">
-      <c r="A27" s="53" t="s">
+      <c r="A27" s="29" t="s">
         <v>174</v>
       </c>
-      <c r="B27" s="54"/>
-      <c r="C27" s="55">
+      <c r="B27" s="3"/>
+      <c r="C27" s="43">
         <v>2023</v>
       </c>
-      <c r="D27" s="56"/>
-      <c r="E27" s="57"/>
-      <c r="F27" s="58"/>
-      <c r="G27" s="58"/>
-      <c r="H27" s="61"/>
-      <c r="I27" s="59"/>
-      <c r="J27" s="58"/>
+      <c r="D27" s="1"/>
+      <c r="E27" s="48"/>
+      <c r="F27" s="11"/>
+      <c r="G27" s="11"/>
+      <c r="H27" s="17"/>
+      <c r="I27" s="42"/>
+      <c r="J27" s="11"/>
     </row>
     <row r="28" spans="1:10" ht="39.6">
-      <c r="A28" s="53" t="s">
+      <c r="A28" s="29" t="s">
         <v>175</v>
       </c>
-      <c r="B28" s="54"/>
-      <c r="C28" s="55"/>
-      <c r="D28" s="56"/>
-      <c r="E28" s="57"/>
-      <c r="F28" s="58"/>
-      <c r="G28" s="58"/>
-      <c r="H28" s="61"/>
-      <c r="I28" s="59"/>
-      <c r="J28" s="58"/>
+      <c r="B28" s="3"/>
+      <c r="C28" s="43"/>
+      <c r="D28" s="1"/>
+      <c r="E28" s="48"/>
+      <c r="F28" s="11"/>
+      <c r="G28" s="11"/>
+      <c r="H28" s="17"/>
+      <c r="I28" s="42"/>
+      <c r="J28" s="11"/>
     </row>
     <row r="29" spans="1:10" ht="39.6">
-      <c r="A29" s="53" t="s">
+      <c r="A29" s="29" t="s">
         <v>176</v>
       </c>
-      <c r="B29" s="54"/>
-      <c r="C29" s="55"/>
-      <c r="D29" s="56"/>
-      <c r="E29" s="57"/>
-      <c r="F29" s="58"/>
-      <c r="G29" s="58"/>
-      <c r="H29" s="61"/>
-      <c r="I29" s="59"/>
-      <c r="J29" s="58"/>
-    </row>
-    <row r="30" spans="1:10" ht="39.6">
-      <c r="A30" s="53" t="s">
+      <c r="B29" s="3"/>
+      <c r="C29" s="43"/>
+      <c r="D29" s="1"/>
+      <c r="E29" s="48"/>
+      <c r="F29" s="11"/>
+      <c r="G29" s="11"/>
+      <c r="H29" s="17"/>
+      <c r="I29" s="42"/>
+      <c r="J29" s="11"/>
+    </row>
+    <row r="30" spans="1:10" ht="26.4">
+      <c r="A30" s="29" t="s">
         <v>177</v>
       </c>
-      <c r="B30" s="54"/>
-      <c r="C30" s="55"/>
-      <c r="D30" s="56"/>
-      <c r="E30" s="57"/>
-      <c r="F30" s="58"/>
-      <c r="G30" s="58"/>
-      <c r="H30" s="61"/>
-      <c r="I30" s="59"/>
-      <c r="J30" s="58"/>
+      <c r="B30" s="3"/>
+      <c r="C30" s="43"/>
+      <c r="D30" s="1"/>
+      <c r="E30" s="48"/>
+      <c r="F30" s="11"/>
+      <c r="G30" s="11"/>
+      <c r="H30" s="17"/>
+      <c r="I30" s="42"/>
+      <c r="J30" s="11"/>
     </row>
     <row r="31" spans="1:10" ht="13.2">
       <c r="A31" s="3"/>

</xml_diff>

<commit_message>
cleaned chinapv_vectorized and pv_china + added the province
</commit_message>
<xml_diff>
--- a/data/BDD.xlsx
+++ b/data/BDD.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\charl\solar-data-china\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5E5FDB03-8EE5-43C7-8BA7-D587E84CD757}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{36AC63D1-6232-459C-A20F-E5F5A767215E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Dataset" sheetId="1" r:id="rId1"/>
@@ -43,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="194" uniqueCount="181">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="200" uniqueCount="187">
   <si>
     <t>Name</t>
   </si>
@@ -839,6 +839,24 @@
   </si>
   <si>
     <t>https://www.pv-magazine.com/2025/06/23/china-hits-1-tw-solar-milestone/</t>
+  </si>
+  <si>
+    <t>https://arxiv.org/abs/2202.01340</t>
+  </si>
+  <si>
+    <t>An Artificial Intelligence Dataset for Solar Energy Locations in India</t>
+  </si>
+  <si>
+    <t>Sebastian Dunnett, Alessandro Sorichetta, Gail Taylor, Feliw Aigenbord</t>
+  </si>
+  <si>
+    <t>Global Renewables Watch website will make derivatives of the data (including the footprint, growth, and estimated total output) available for download on GitHub. -&gt; not found</t>
+  </si>
+  <si>
+    <t>https://figshare.com/articles/dataset/Harmonised_global_datasets_of_wind_and_solar_farm_locations_and_power/11310269?file=23348810</t>
+  </si>
+  <si>
+    <t>https://github.com/microsoft/solar-farms-mapping?tab=readme-ov-file</t>
   </si>
 </sst>
 </file>
@@ -1040,7 +1058,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="54">
+  <cellXfs count="60">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -1146,9 +1164,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
@@ -1186,8 +1201,27 @@
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="1"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="1" applyAlignment="1">
-      <alignment wrapText="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1684,7 +1718,7 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{00000000-000C-0000-FFFF-FFFF01000000}" name="Articles" displayName="Articles" ref="A1:J30" headerRowDxfId="15" dataDxfId="14" totalsRowDxfId="13">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{00000000-000C-0000-FFFF-FFFF01000000}" name="Articles" displayName="Articles" ref="A1:J31" headerRowDxfId="15" dataDxfId="14" totalsRowDxfId="13">
   <tableColumns count="10">
     <tableColumn id="1" xr3:uid="{00000000-0010-0000-0100-000001000000}" name="Title " dataDxfId="12"/>
     <tableColumn id="2" xr3:uid="{00000000-0010-0000-0100-000002000000}" name="Author " dataDxfId="11"/>
@@ -1904,11 +1938,11 @@
   </sheetPr>
   <dimension ref="A1:O47"/>
   <sheetViews>
-    <sheetView zoomScale="66" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B16" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" zoomScale="66" zoomScaleNormal="100" workbookViewId="0">
+      <pane xSplit="1" ySplit="1" topLeftCell="E2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="H36" sqref="H36"/>
+      <selection pane="bottomRight" activeCell="K2" sqref="K2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1"/>
@@ -1930,43 +1964,43 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:15" s="15" customFormat="1" ht="13.8">
-      <c r="A1" s="44" t="s">
+      <c r="A1" s="43" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="45" t="s">
+      <c r="B1" s="44" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="44" t="s">
+      <c r="C1" s="43" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="46" t="s">
+      <c r="D1" s="45" t="s">
         <v>90</v>
       </c>
-      <c r="E1" s="44" t="s">
+      <c r="E1" s="43" t="s">
         <v>94</v>
       </c>
-      <c r="F1" s="44" t="s">
+      <c r="F1" s="43" t="s">
         <v>4</v>
       </c>
-      <c r="G1" s="46" t="s">
+      <c r="G1" s="45" t="s">
         <v>5</v>
       </c>
-      <c r="H1" s="44" t="s">
+      <c r="H1" s="43" t="s">
         <v>6</v>
       </c>
-      <c r="I1" s="46" t="s">
+      <c r="I1" s="45" t="s">
         <v>7</v>
       </c>
-      <c r="J1" s="44" t="s">
+      <c r="J1" s="43" t="s">
         <v>8</v>
       </c>
-      <c r="K1" s="44" t="s">
+      <c r="K1" s="43" t="s">
         <v>9</v>
       </c>
-      <c r="L1" s="45" t="s">
+      <c r="L1" s="44" t="s">
         <v>10</v>
       </c>
-      <c r="M1" s="44" t="s">
+      <c r="M1" s="43" t="s">
         <v>11</v>
       </c>
       <c r="N1" s="15" t="s">
@@ -2512,7 +2546,7 @@
       <c r="C30" s="19" t="s">
         <v>40</v>
       </c>
-      <c r="D30" s="52" t="s">
+      <c r="D30" s="51" t="s">
         <v>41</v>
       </c>
       <c r="E30" s="2"/>
@@ -2797,11 +2831,11 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:L1002"/>
+  <dimension ref="A1:L1003"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3" zoomScale="76" zoomScaleNormal="106" workbookViewId="0">
-      <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="F3" sqref="F3"/>
+    <sheetView topLeftCell="A2" zoomScale="73" zoomScaleNormal="106" workbookViewId="0">
+      <pane xSplit="1" topLeftCell="F1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="H3" sqref="H3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1"/>
@@ -2810,7 +2844,7 @@
     <col min="2" max="2" width="23" customWidth="1"/>
     <col min="3" max="3" width="15.109375" customWidth="1"/>
     <col min="4" max="4" width="18.77734375" customWidth="1"/>
-    <col min="5" max="5" width="21.6640625" style="47" customWidth="1"/>
+    <col min="5" max="5" width="21.6640625" style="46" customWidth="1"/>
     <col min="6" max="6" width="100.77734375" customWidth="1"/>
     <col min="7" max="7" width="23.77734375" customWidth="1"/>
     <col min="8" max="8" width="13" customWidth="1"/>
@@ -2928,7 +2962,7 @@
       <c r="D4" s="3" t="s">
         <v>88</v>
       </c>
-      <c r="E4" s="40" t="s">
+      <c r="E4" s="39" t="s">
         <v>129</v>
       </c>
       <c r="F4" s="3" t="s">
@@ -2946,13 +2980,13 @@
       </c>
     </row>
     <row r="5" spans="1:12" ht="92.4">
-      <c r="A5" s="51" t="s">
+      <c r="A5" s="50" t="s">
         <v>118</v>
       </c>
       <c r="B5" s="3" t="s">
         <v>115</v>
       </c>
-      <c r="C5" s="41" t="s">
+      <c r="C5" s="40" t="s">
         <v>116</v>
       </c>
       <c r="D5" s="18"/>
@@ -2962,401 +2996,422 @@
       <c r="F5" s="11"/>
       <c r="G5" s="11"/>
       <c r="H5" s="17"/>
-      <c r="I5" s="42"/>
-      <c r="J5" s="11"/>
-    </row>
-    <row r="6" spans="1:12" ht="52.8">
-      <c r="A6" s="29" t="s">
-        <v>122</v>
-      </c>
-      <c r="B6" s="3" t="s">
-        <v>123</v>
-      </c>
-      <c r="C6" s="43">
-        <v>2021</v>
-      </c>
-      <c r="D6" s="12" t="s">
-        <v>124</v>
-      </c>
-      <c r="E6" s="16" t="s">
-        <v>121</v>
-      </c>
-      <c r="F6" s="11"/>
-      <c r="G6" s="11"/>
-      <c r="H6" s="17"/>
-      <c r="I6" s="42"/>
-      <c r="J6" s="11"/>
+      <c r="I5" s="41"/>
+      <c r="J5" s="18" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" ht="26.4">
+      <c r="A6" s="53" t="s">
+        <v>182</v>
+      </c>
+      <c r="B6" s="58"/>
+      <c r="C6" s="59"/>
+      <c r="D6" s="55"/>
+      <c r="E6" s="37" t="s">
+        <v>181</v>
+      </c>
+      <c r="F6" s="56"/>
+      <c r="G6" s="56"/>
+      <c r="H6" s="16" t="s">
+        <v>186</v>
+      </c>
+      <c r="I6" s="57"/>
+      <c r="J6" s="56"/>
     </row>
     <row r="7" spans="1:12" ht="52.8">
       <c r="A7" s="29" t="s">
-        <v>132</v>
-      </c>
-      <c r="B7" s="3"/>
-      <c r="C7" s="43"/>
-      <c r="D7" s="1"/>
+        <v>122</v>
+      </c>
+      <c r="B7" s="3" t="s">
+        <v>123</v>
+      </c>
+      <c r="C7" s="42">
+        <v>2021</v>
+      </c>
+      <c r="D7" s="12" t="s">
+        <v>124</v>
+      </c>
       <c r="E7" s="16" t="s">
-        <v>146</v>
+        <v>121</v>
       </c>
       <c r="F7" s="11"/>
       <c r="G7" s="11"/>
-      <c r="H7" s="53" t="s">
+      <c r="H7" s="17"/>
+      <c r="I7" s="41"/>
+      <c r="J7" s="11"/>
+    </row>
+    <row r="8" spans="1:12" ht="39.6">
+      <c r="A8" s="29" t="s">
+        <v>132</v>
+      </c>
+      <c r="B8" s="3"/>
+      <c r="C8" s="42"/>
+      <c r="D8" s="1"/>
+      <c r="E8" s="16" t="s">
+        <v>146</v>
+      </c>
+      <c r="F8" s="11"/>
+      <c r="G8" s="11"/>
+      <c r="H8" s="39" t="s">
         <v>147</v>
       </c>
-      <c r="I7" s="42"/>
-      <c r="J7" s="52" t="s">
+      <c r="I8" s="41"/>
+      <c r="J8" s="39" t="s">
         <v>133</v>
       </c>
     </row>
-    <row r="8" spans="1:12" ht="39.6">
-      <c r="A8" s="31" t="s">
+    <row r="9" spans="1:12" ht="39.6">
+      <c r="A9" s="31" t="s">
         <v>149</v>
       </c>
-      <c r="B8" s="47"/>
-      <c r="E8" s="40" t="s">
+      <c r="B9" s="46"/>
+      <c r="E9" s="39" t="s">
         <v>148</v>
       </c>
-      <c r="H8" s="38"/>
-    </row>
-    <row r="9" spans="1:12" ht="26.4">
-      <c r="A9" s="29" t="s">
-        <v>135</v>
-      </c>
-      <c r="B9" s="3"/>
-      <c r="C9" s="43"/>
-      <c r="D9" s="1"/>
-      <c r="E9" s="16" t="s">
-        <v>134</v>
-      </c>
-      <c r="F9" s="11"/>
-      <c r="G9" s="11"/>
-      <c r="H9" s="17"/>
-      <c r="I9" s="42"/>
-      <c r="J9" s="11"/>
+      <c r="H9" s="38"/>
     </row>
     <row r="10" spans="1:12" ht="52.8">
-      <c r="A10" s="29" t="s">
-        <v>136</v>
-      </c>
-      <c r="B10" s="3"/>
-      <c r="C10" s="43"/>
+      <c r="A10" s="48" t="s">
+        <v>157</v>
+      </c>
+      <c r="B10" s="52" t="s">
+        <v>183</v>
+      </c>
+      <c r="C10" s="54">
+        <v>2020</v>
+      </c>
       <c r="D10" s="1"/>
       <c r="E10" s="16" t="s">
-        <v>137</v>
+        <v>158</v>
       </c>
       <c r="F10" s="11"/>
       <c r="G10" s="11"/>
-      <c r="H10" s="17"/>
-      <c r="I10" s="42"/>
+      <c r="H10" s="39" t="s">
+        <v>185</v>
+      </c>
+      <c r="I10" s="41"/>
       <c r="J10" s="11"/>
     </row>
-    <row r="11" spans="1:12" ht="39.6">
-      <c r="A11" s="49" t="s">
-        <v>138</v>
+    <row r="11" spans="1:12" ht="26.4">
+      <c r="A11" s="29" t="s">
+        <v>135</v>
       </c>
       <c r="B11" s="3"/>
-      <c r="C11" s="43"/>
+      <c r="C11" s="42"/>
       <c r="D11" s="1"/>
       <c r="E11" s="16" t="s">
-        <v>139</v>
+        <v>134</v>
       </c>
       <c r="F11" s="11"/>
       <c r="G11" s="11"/>
       <c r="H11" s="17"/>
-      <c r="I11" s="42"/>
+      <c r="I11" s="41"/>
       <c r="J11" s="11"/>
     </row>
     <row r="12" spans="1:12" ht="52.8">
-      <c r="A12" s="49" t="s">
-        <v>140</v>
+      <c r="A12" s="29" t="s">
+        <v>136</v>
       </c>
       <c r="B12" s="3"/>
-      <c r="C12" s="43"/>
+      <c r="C12" s="42"/>
       <c r="D12" s="1"/>
       <c r="E12" s="16" t="s">
-        <v>141</v>
+        <v>137</v>
       </c>
       <c r="F12" s="11"/>
       <c r="G12" s="11"/>
       <c r="H12" s="17"/>
-      <c r="I12" s="42"/>
+      <c r="I12" s="41"/>
       <c r="J12" s="11"/>
     </row>
     <row r="13" spans="1:12" ht="39.6">
-      <c r="A13" s="49" t="s">
-        <v>142</v>
+      <c r="A13" s="48" t="s">
+        <v>138</v>
       </c>
       <c r="B13" s="3"/>
-      <c r="C13" s="43"/>
+      <c r="C13" s="42"/>
       <c r="D13" s="1"/>
       <c r="E13" s="16" t="s">
-        <v>143</v>
+        <v>139</v>
       </c>
       <c r="F13" s="11"/>
       <c r="G13" s="11"/>
       <c r="H13" s="17"/>
-      <c r="I13" s="42"/>
+      <c r="I13" s="41"/>
       <c r="J13" s="11"/>
     </row>
-    <row r="14" spans="1:12" ht="39.6">
-      <c r="A14" s="49" t="s">
-        <v>144</v>
+    <row r="14" spans="1:12" ht="52.8">
+      <c r="A14" s="48" t="s">
+        <v>140</v>
       </c>
       <c r="B14" s="3"/>
-      <c r="C14" s="43"/>
+      <c r="C14" s="42"/>
       <c r="D14" s="1"/>
       <c r="E14" s="16" t="s">
-        <v>145</v>
+        <v>141</v>
       </c>
       <c r="F14" s="11"/>
       <c r="G14" s="11"/>
       <c r="H14" s="17"/>
-      <c r="I14" s="42"/>
+      <c r="I14" s="41"/>
       <c r="J14" s="11"/>
     </row>
     <row r="15" spans="1:12" ht="39.6">
-      <c r="A15" s="49" t="s">
-        <v>150</v>
+      <c r="A15" s="48" t="s">
+        <v>142</v>
       </c>
       <c r="B15" s="3"/>
-      <c r="C15" s="43"/>
+      <c r="C15" s="42"/>
       <c r="D15" s="1"/>
       <c r="E15" s="16" t="s">
-        <v>151</v>
+        <v>143</v>
       </c>
       <c r="F15" s="11"/>
       <c r="G15" s="11"/>
       <c r="H15" s="17"/>
-      <c r="I15" s="42"/>
+      <c r="I15" s="41"/>
       <c r="J15" s="11"/>
     </row>
-    <row r="16" spans="1:12" ht="26.4">
-      <c r="A16" s="29" t="s">
-        <v>152</v>
+    <row r="16" spans="1:12" ht="39.6">
+      <c r="A16" s="48" t="s">
+        <v>144</v>
       </c>
       <c r="B16" s="3"/>
-      <c r="C16" s="43"/>
+      <c r="C16" s="42"/>
       <c r="D16" s="1"/>
       <c r="E16" s="16" t="s">
-        <v>153</v>
+        <v>145</v>
       </c>
       <c r="F16" s="11"/>
       <c r="G16" s="11"/>
       <c r="H16" s="17"/>
-      <c r="I16" s="42"/>
+      <c r="I16" s="41"/>
       <c r="J16" s="11"/>
     </row>
-    <row r="17" spans="1:10" ht="26.4">
-      <c r="A17" s="50" t="s">
-        <v>154</v>
+    <row r="17" spans="1:10" ht="39.6">
+      <c r="A17" s="48" t="s">
+        <v>150</v>
       </c>
       <c r="B17" s="3"/>
-      <c r="C17" s="43"/>
+      <c r="C17" s="42"/>
       <c r="D17" s="1"/>
       <c r="E17" s="16" t="s">
-        <v>155</v>
+        <v>151</v>
       </c>
       <c r="F17" s="11"/>
       <c r="G17" s="11"/>
       <c r="H17" s="17"/>
-      <c r="I17" s="42"/>
+      <c r="I17" s="41"/>
       <c r="J17" s="11"/>
     </row>
-    <row r="18" spans="1:10" ht="39.6">
-      <c r="A18" s="50" t="s">
-        <v>156</v>
+    <row r="18" spans="1:10" ht="26.4">
+      <c r="A18" s="29" t="s">
+        <v>152</v>
       </c>
       <c r="B18" s="3"/>
-      <c r="C18" s="43"/>
+      <c r="C18" s="42"/>
       <c r="D18" s="1"/>
       <c r="E18" s="16" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="F18" s="11"/>
       <c r="G18" s="11"/>
       <c r="H18" s="17"/>
-      <c r="I18" s="42"/>
+      <c r="I18" s="41"/>
       <c r="J18" s="11"/>
     </row>
     <row r="19" spans="1:10" ht="26.4">
       <c r="A19" s="49" t="s">
-        <v>157</v>
+        <v>154</v>
       </c>
       <c r="B19" s="3"/>
-      <c r="C19" s="43"/>
+      <c r="C19" s="42"/>
       <c r="D19" s="1"/>
       <c r="E19" s="16" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
       <c r="F19" s="11"/>
       <c r="G19" s="11"/>
       <c r="H19" s="17"/>
-      <c r="I19" s="42"/>
+      <c r="I19" s="41"/>
       <c r="J19" s="11"/>
     </row>
-    <row r="20" spans="1:10" ht="39.6">
+    <row r="20" spans="1:10" ht="55.2" customHeight="1">
       <c r="A20" s="49" t="s">
-        <v>159</v>
+        <v>156</v>
       </c>
       <c r="B20" s="3"/>
-      <c r="C20" s="43"/>
+      <c r="C20" s="42"/>
       <c r="D20" s="1"/>
       <c r="E20" s="16" t="s">
-        <v>160</v>
+        <v>155</v>
       </c>
       <c r="F20" s="11"/>
       <c r="G20" s="11"/>
       <c r="H20" s="17"/>
-      <c r="I20" s="42"/>
+      <c r="I20" s="41"/>
       <c r="J20" s="11"/>
     </row>
     <row r="21" spans="1:10" ht="55.2" customHeight="1">
-      <c r="A21" s="50" t="s">
-        <v>161</v>
+      <c r="A21" s="48" t="s">
+        <v>159</v>
       </c>
       <c r="B21" s="3"/>
-      <c r="C21" s="43"/>
+      <c r="C21" s="42"/>
       <c r="D21" s="1"/>
-      <c r="E21" s="48"/>
+      <c r="E21" s="16" t="s">
+        <v>160</v>
+      </c>
       <c r="F21" s="11"/>
       <c r="G21" s="11"/>
       <c r="H21" s="17"/>
-      <c r="I21" s="42"/>
+      <c r="I21" s="41"/>
       <c r="J21" s="11"/>
     </row>
-    <row r="22" spans="1:10" ht="30.6" customHeight="1">
-      <c r="A22" s="50" t="s">
-        <v>162</v>
+    <row r="22" spans="1:10" ht="39.6">
+      <c r="A22" s="49" t="s">
+        <v>161</v>
       </c>
       <c r="B22" s="3"/>
-      <c r="C22" s="43"/>
+      <c r="C22" s="42"/>
       <c r="D22" s="1"/>
-      <c r="E22" s="48"/>
+      <c r="E22" s="47"/>
       <c r="F22" s="11"/>
       <c r="G22" s="11"/>
       <c r="H22" s="17"/>
-      <c r="I22" s="42"/>
+      <c r="I22" s="41"/>
       <c r="J22" s="11"/>
     </row>
-    <row r="23" spans="1:10" ht="52.8">
-      <c r="A23" s="50" t="s">
-        <v>163</v>
+    <row r="23" spans="1:10" ht="26.4">
+      <c r="A23" s="49" t="s">
+        <v>162</v>
       </c>
       <c r="B23" s="3"/>
-      <c r="C23" s="43"/>
+      <c r="C23" s="42"/>
       <c r="D23" s="1"/>
-      <c r="E23" s="48"/>
+      <c r="E23" s="47"/>
       <c r="F23" s="11"/>
       <c r="G23" s="11"/>
       <c r="H23" s="17"/>
-      <c r="I23" s="42"/>
+      <c r="I23" s="41"/>
       <c r="J23" s="11"/>
     </row>
-    <row r="24" spans="1:10" ht="39.6">
+    <row r="24" spans="1:10" ht="52.8">
       <c r="A24" s="49" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="B24" s="3"/>
-      <c r="C24" s="43"/>
+      <c r="C24" s="42"/>
       <c r="D24" s="1"/>
-      <c r="E24" s="16" t="s">
-        <v>165</v>
-      </c>
+      <c r="E24" s="47"/>
       <c r="F24" s="11"/>
       <c r="G24" s="11"/>
       <c r="H24" s="17"/>
-      <c r="I24" s="42"/>
+      <c r="I24" s="41"/>
       <c r="J24" s="11"/>
     </row>
-    <row r="25" spans="1:10" ht="26.4">
-      <c r="A25" s="29" t="s">
-        <v>169</v>
+    <row r="25" spans="1:10" ht="39.6">
+      <c r="A25" s="48" t="s">
+        <v>164</v>
       </c>
       <c r="B25" s="3"/>
-      <c r="C25" s="43"/>
+      <c r="C25" s="42"/>
       <c r="D25" s="1"/>
-      <c r="E25" s="48"/>
+      <c r="E25" s="16" t="s">
+        <v>165</v>
+      </c>
       <c r="F25" s="11"/>
       <c r="G25" s="11"/>
       <c r="H25" s="17"/>
-      <c r="I25" s="42"/>
+      <c r="I25" s="41"/>
       <c r="J25" s="11"/>
     </row>
-    <row r="26" spans="1:10" ht="39.6">
+    <row r="26" spans="1:10" ht="26.4">
       <c r="A26" s="29" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="B26" s="3"/>
-      <c r="C26" s="43"/>
+      <c r="C26" s="42"/>
       <c r="D26" s="1"/>
-      <c r="E26" s="48"/>
+      <c r="E26" s="47"/>
       <c r="F26" s="11"/>
       <c r="G26" s="11"/>
       <c r="H26" s="17"/>
-      <c r="I26" s="42"/>
+      <c r="I26" s="41"/>
       <c r="J26" s="11"/>
     </row>
-    <row r="27" spans="1:10" ht="52.8">
+    <row r="27" spans="1:10" ht="39.6">
       <c r="A27" s="29" t="s">
-        <v>174</v>
+        <v>170</v>
       </c>
       <c r="B27" s="3"/>
-      <c r="C27" s="43">
-        <v>2023</v>
-      </c>
+      <c r="C27" s="42"/>
       <c r="D27" s="1"/>
-      <c r="E27" s="48"/>
+      <c r="E27" s="47"/>
       <c r="F27" s="11"/>
       <c r="G27" s="11"/>
       <c r="H27" s="17"/>
-      <c r="I27" s="42"/>
+      <c r="I27" s="41"/>
       <c r="J27" s="11"/>
     </row>
-    <row r="28" spans="1:10" ht="39.6">
+    <row r="28" spans="1:10" ht="52.8">
       <c r="A28" s="29" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="B28" s="3"/>
-      <c r="C28" s="43"/>
+      <c r="C28" s="42">
+        <v>2023</v>
+      </c>
       <c r="D28" s="1"/>
-      <c r="E28" s="48"/>
+      <c r="E28" s="47"/>
       <c r="F28" s="11"/>
       <c r="G28" s="11"/>
       <c r="H28" s="17"/>
-      <c r="I28" s="42"/>
+      <c r="I28" s="41"/>
       <c r="J28" s="11"/>
     </row>
     <row r="29" spans="1:10" ht="39.6">
       <c r="A29" s="29" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="B29" s="3"/>
-      <c r="C29" s="43"/>
+      <c r="C29" s="42"/>
       <c r="D29" s="1"/>
-      <c r="E29" s="48"/>
+      <c r="E29" s="47"/>
       <c r="F29" s="11"/>
       <c r="G29" s="11"/>
       <c r="H29" s="17"/>
-      <c r="I29" s="42"/>
+      <c r="I29" s="41"/>
       <c r="J29" s="11"/>
     </row>
-    <row r="30" spans="1:10" ht="26.4">
+    <row r="30" spans="1:10" ht="39.6">
       <c r="A30" s="29" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="B30" s="3"/>
-      <c r="C30" s="43"/>
+      <c r="C30" s="42"/>
       <c r="D30" s="1"/>
-      <c r="E30" s="48"/>
+      <c r="E30" s="47"/>
       <c r="F30" s="11"/>
       <c r="G30" s="11"/>
       <c r="H30" s="17"/>
-      <c r="I30" s="42"/>
+      <c r="I30" s="41"/>
       <c r="J30" s="11"/>
     </row>
-    <row r="31" spans="1:10" ht="13.2">
-      <c r="A31" s="3"/>
-      <c r="B31" s="1"/>
+    <row r="31" spans="1:10" ht="26.4">
+      <c r="A31" s="29" t="s">
+        <v>177</v>
+      </c>
+      <c r="B31" s="3"/>
+      <c r="C31" s="42"/>
       <c r="D31" s="1"/>
+      <c r="E31" s="47"/>
+      <c r="F31" s="11"/>
+      <c r="G31" s="11"/>
+      <c r="H31" s="17"/>
+      <c r="I31" s="41"/>
+      <c r="J31" s="11"/>
     </row>
     <row r="32" spans="1:10" ht="13.2">
       <c r="A32" s="3"/>
@@ -8212,6 +8267,11 @@
       <c r="A1002" s="3"/>
       <c r="B1002" s="1"/>
       <c r="D1002" s="1"/>
+    </row>
+    <row r="1003" spans="1:4" ht="15.75" customHeight="1">
+      <c r="A1003" s="3"/>
+      <c r="B1003" s="1"/>
+      <c r="D1003" s="1"/>
     </row>
   </sheetData>
   <hyperlinks>
@@ -8220,30 +8280,33 @@
     <hyperlink ref="E4" r:id="rId3" xr:uid="{00000000-0004-0000-0100-000002000000}"/>
     <hyperlink ref="E5" r:id="rId4" xr:uid="{2CB38D27-E0A1-4F65-9CE4-CD7061C110B5}"/>
     <hyperlink ref="H2" r:id="rId5" xr:uid="{7C11FBB4-777B-4890-848E-C9942EB60B3A}"/>
-    <hyperlink ref="E6" r:id="rId6" xr:uid="{F07B1B6C-925F-45B7-ADA2-66DB99A70D32}"/>
-    <hyperlink ref="E7" r:id="rId7" xr:uid="{2C87EC1D-8884-4C1F-8FF0-BAD119A8A368}"/>
-    <hyperlink ref="E9" r:id="rId8" xr:uid="{5907EA6F-1CF1-4DF9-8994-FBA5AD8346F7}"/>
-    <hyperlink ref="E10" r:id="rId9" xr:uid="{1DD4506C-73B7-4DB3-84B5-1D3589E736DE}"/>
-    <hyperlink ref="E11" r:id="rId10" xr:uid="{4DA94359-7D56-4240-8E42-31CBF23D6FF5}"/>
-    <hyperlink ref="E12" r:id="rId11" xr:uid="{ACE9DE55-96B2-44FF-9CE2-2E5818FC9998}"/>
-    <hyperlink ref="E13" r:id="rId12" xr:uid="{6BBD425B-D522-4BAF-B046-4BC871730270}"/>
-    <hyperlink ref="E14" r:id="rId13" xr:uid="{155DE230-543F-4889-B5AE-6FA49A6D08BA}"/>
-    <hyperlink ref="E8" r:id="rId14" xr:uid="{63B4D8F1-870B-44AA-A576-089679578BE1}"/>
-    <hyperlink ref="E15" r:id="rId15" xr:uid="{55A59522-8FBD-4A43-B576-D4CE614341D7}"/>
-    <hyperlink ref="E16" r:id="rId16" xr:uid="{5B989690-003F-4923-B7F4-A47A85945677}"/>
-    <hyperlink ref="E17" r:id="rId17" xr:uid="{1F44A843-12CF-4E9B-A153-243927E180AA}"/>
-    <hyperlink ref="E18" r:id="rId18" xr:uid="{E206D339-90EF-431C-A40C-1EA010BA239D}"/>
-    <hyperlink ref="E19" r:id="rId19" xr:uid="{F9100E57-6F7E-4BBD-91B2-826029FEB248}"/>
-    <hyperlink ref="E20" r:id="rId20" xr:uid="{766864F1-8314-4690-BDD1-403D573EE1A2}"/>
-    <hyperlink ref="E24" r:id="rId21" xr:uid="{7243A186-84D9-4A2B-A3C9-2D8B161DBD81}"/>
-    <hyperlink ref="H7" r:id="rId22" xr:uid="{5AF6AD83-A0DB-402A-9E62-981A344C4043}"/>
-    <hyperlink ref="J7" r:id="rId23" xr:uid="{1438E023-47FA-4020-9EE1-A00F3090FF72}"/>
+    <hyperlink ref="E7" r:id="rId6" xr:uid="{F07B1B6C-925F-45B7-ADA2-66DB99A70D32}"/>
+    <hyperlink ref="E8" r:id="rId7" xr:uid="{2C87EC1D-8884-4C1F-8FF0-BAD119A8A368}"/>
+    <hyperlink ref="E11" r:id="rId8" xr:uid="{5907EA6F-1CF1-4DF9-8994-FBA5AD8346F7}"/>
+    <hyperlink ref="E12" r:id="rId9" xr:uid="{1DD4506C-73B7-4DB3-84B5-1D3589E736DE}"/>
+    <hyperlink ref="E13" r:id="rId10" xr:uid="{4DA94359-7D56-4240-8E42-31CBF23D6FF5}"/>
+    <hyperlink ref="E14" r:id="rId11" xr:uid="{ACE9DE55-96B2-44FF-9CE2-2E5818FC9998}"/>
+    <hyperlink ref="E15" r:id="rId12" xr:uid="{6BBD425B-D522-4BAF-B046-4BC871730270}"/>
+    <hyperlink ref="E16" r:id="rId13" xr:uid="{155DE230-543F-4889-B5AE-6FA49A6D08BA}"/>
+    <hyperlink ref="E9" r:id="rId14" xr:uid="{63B4D8F1-870B-44AA-A576-089679578BE1}"/>
+    <hyperlink ref="E17" r:id="rId15" xr:uid="{55A59522-8FBD-4A43-B576-D4CE614341D7}"/>
+    <hyperlink ref="E18" r:id="rId16" xr:uid="{5B989690-003F-4923-B7F4-A47A85945677}"/>
+    <hyperlink ref="E19" r:id="rId17" xr:uid="{1F44A843-12CF-4E9B-A153-243927E180AA}"/>
+    <hyperlink ref="E20" r:id="rId18" xr:uid="{E206D339-90EF-431C-A40C-1EA010BA239D}"/>
+    <hyperlink ref="E10" r:id="rId19" xr:uid="{F9100E57-6F7E-4BBD-91B2-826029FEB248}"/>
+    <hyperlink ref="E21" r:id="rId20" xr:uid="{766864F1-8314-4690-BDD1-403D573EE1A2}"/>
+    <hyperlink ref="E25" r:id="rId21" xr:uid="{7243A186-84D9-4A2B-A3C9-2D8B161DBD81}"/>
+    <hyperlink ref="H8" r:id="rId22" xr:uid="{5AF6AD83-A0DB-402A-9E62-981A344C4043}"/>
+    <hyperlink ref="J8" r:id="rId23" xr:uid="{1438E023-47FA-4020-9EE1-A00F3090FF72}"/>
     <hyperlink ref="H3" r:id="rId24" display="https://zenodo.org/records/14292571" xr:uid="{B8E688FD-5EF4-4175-B267-588646FB1807}"/>
+    <hyperlink ref="E6" r:id="rId25" xr:uid="{3AC147B4-BB92-4910-8D62-00FDAADC05B1}"/>
+    <hyperlink ref="H10" r:id="rId26" xr:uid="{8E9BCBE4-EEA1-4B02-B7E5-3B46AEA87B92}"/>
+    <hyperlink ref="H6" r:id="rId27" xr:uid="{8F125A05-13A9-4DD6-ABFD-E7C8A8884495}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId25"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId28"/>
   <tableParts count="1">
-    <tablePart r:id="rId26"/>
+    <tablePart r:id="rId29"/>
   </tableParts>
 </worksheet>
 </file>
@@ -8259,7 +8322,7 @@
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13.2"/>
   <sheetData>
     <row r="1" spans="1:1">
-      <c r="A1" s="52" t="s">
+      <c r="A1" s="51" t="s">
         <v>179</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Comparaison of the 3 datasets
</commit_message>
<xml_diff>
--- a/data/BDD.xlsx
+++ b/data/BDD.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\charl\solar-data-china\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{36AC63D1-6232-459C-A20F-E5F5A767215E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D9445F83-A402-4F51-AE8E-4B954BD4C1ED}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Dataset" sheetId="1" r:id="rId1"/>
@@ -1058,7 +1058,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="60">
+  <cellXfs count="52">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -1201,28 +1201,6 @@
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Lien hypertexte" xfId="1" builtinId="8"/>
@@ -1938,7 +1916,7 @@
   </sheetPr>
   <dimension ref="A1:O47"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="66" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScale="66" zoomScaleNormal="100" workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="E2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
@@ -2161,7 +2139,7 @@
       </c>
       <c r="O5" s="18"/>
     </row>
-    <row r="6" spans="1:15" ht="184.8">
+    <row r="6" spans="1:15" ht="198">
       <c r="A6" s="2" t="s">
         <v>35</v>
       </c>
@@ -2833,8 +2811,8 @@
   </sheetPr>
   <dimension ref="A1:L1003"/>
   <sheetViews>
-    <sheetView topLeftCell="A2" zoomScale="73" zoomScaleNormal="106" workbookViewId="0">
-      <pane xSplit="1" topLeftCell="F1" activePane="topRight" state="frozen"/>
+    <sheetView tabSelected="1" topLeftCell="A2" zoomScale="73" zoomScaleNormal="106" workbookViewId="0">
+      <pane xSplit="1" topLeftCell="E1" activePane="topRight" state="frozen"/>
       <selection pane="topRight" activeCell="H3" sqref="H3"/>
     </sheetView>
   </sheetViews>
@@ -3002,22 +2980,22 @@
       </c>
     </row>
     <row r="6" spans="1:12" ht="26.4">
-      <c r="A6" s="53" t="s">
+      <c r="A6" s="50" t="s">
         <v>182</v>
       </c>
-      <c r="B6" s="58"/>
-      <c r="C6" s="59"/>
-      <c r="D6" s="55"/>
+      <c r="B6" s="47"/>
+      <c r="C6" s="42"/>
+      <c r="D6" s="18"/>
       <c r="E6" s="37" t="s">
         <v>181</v>
       </c>
-      <c r="F6" s="56"/>
-      <c r="G6" s="56"/>
+      <c r="F6" s="11"/>
+      <c r="G6" s="11"/>
       <c r="H6" s="16" t="s">
         <v>186</v>
       </c>
-      <c r="I6" s="57"/>
-      <c r="J6" s="56"/>
+      <c r="I6" s="41"/>
+      <c r="J6" s="11"/>
     </row>
     <row r="7" spans="1:12" ht="52.8">
       <c r="A7" s="29" t="s">
@@ -3075,10 +3053,10 @@
       <c r="A10" s="48" t="s">
         <v>157</v>
       </c>
-      <c r="B10" s="52" t="s">
+      <c r="B10" s="3" t="s">
         <v>183</v>
       </c>
-      <c r="C10" s="54">
+      <c r="C10" s="40">
         <v>2020</v>
       </c>
       <c r="D10" s="1"/>
@@ -3399,7 +3377,7 @@
       <c r="I30" s="41"/>
       <c r="J30" s="11"/>
     </row>
-    <row r="31" spans="1:10" ht="26.4">
+    <row r="31" spans="1:10" ht="39.6">
       <c r="A31" s="29" t="s">
         <v>177</v>
       </c>

</xml_diff>

<commit_message>
Finished the comparaison analysis
</commit_message>
<xml_diff>
--- a/data/BDD.xlsx
+++ b/data/BDD.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\charl\solar-data-china\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D9445F83-A402-4F51-AE8E-4B954BD4C1ED}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EA6A8BB8-86EF-4A09-9570-FAE8105F7199}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -2811,8 +2811,8 @@
   </sheetPr>
   <dimension ref="A1:L1003"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" zoomScale="73" zoomScaleNormal="106" workbookViewId="0">
-      <pane xSplit="1" topLeftCell="E1" activePane="topRight" state="frozen"/>
+    <sheetView tabSelected="1" topLeftCell="A21" zoomScale="73" zoomScaleNormal="106" workbookViewId="0">
+      <pane xSplit="1" topLeftCell="C1" activePane="topRight" state="frozen"/>
       <selection pane="topRight" activeCell="H3" sqref="H3"/>
     </sheetView>
   </sheetViews>

</xml_diff>